<commit_message>
final version of Excel spreadsheet for comparison
</commit_message>
<xml_diff>
--- a/notebooks/data/esoph-tab.xlsx
+++ b/notebooks/data/esoph-tab.xlsx
@@ -8,19 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lpritc/Library/Mobile Documents/com~apple~CloudDocs/Strathclyde_Teaching_iCloud/2021-2022/BM432/BM432/notebooks/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E3DDF7AE-E3F4-6447-B0EA-CF02FA6A37CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{7E6B309E-92AD-DF4C-BA9D-EFD0171DCBB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="64380" yWindow="16960" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="60280" yWindow="-4020" windowWidth="28040" windowHeight="17440"/>
   </bookViews>
   <sheets>
-    <sheet name="esoph-tab" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="esoph-tab" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
+  <pivotCaches>
+    <pivotCache cacheId="3" r:id="rId3"/>
+  </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="25">
   <si>
     <t>agegp</t>
   </si>
@@ -46,49 +50,19 @@
     <t>0-9</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
     <t>10-19</t>
-  </si>
-  <si>
-    <t>10</t>
   </si>
   <si>
     <t>20-29</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
     <t>30+</t>
-  </si>
-  <si>
-    <t>5</t>
   </si>
   <si>
     <t>40-79</t>
   </si>
   <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>80-119</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
   <si>
     <t>120+</t>
@@ -97,79 +71,34 @@
     <t>35-44</t>
   </si>
   <si>
-    <t>60</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
     <t>45-54</t>
-  </si>
-  <si>
-    <t>46</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>16</t>
   </si>
   <si>
     <t>55-64</t>
   </si>
   <si>
-    <t>49</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
     <t>65-74</t>
   </si>
   <si>
-    <t>48</t>
+    <t>75+</t>
   </si>
   <si>
-    <t>34</t>
+    <t>Mean:</t>
   </si>
   <si>
-    <t>13</t>
+    <t>Std Dev:</t>
   </si>
   <si>
-    <t>75+</t>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Sum of ncases</t>
+  </si>
+  <si>
+    <t>Sum of ncontrols</t>
   </si>
 </sst>
 </file>
@@ -653,9 +582,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -712,6 +646,1844 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[esoph-tab.xlsx]Sheet1!PivotTable1</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sum of ncases</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$4:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0-39</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>120+</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40-79</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80-119</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>51</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8BF3-B246-948F-32C3FE9DE6DC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sum of ncontrols</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$4:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0-39</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>120+</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40-79</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80-119</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$4:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>415</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>355</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>138</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8BF3-B246-948F-32C3FE9DE6DC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1314612192"/>
+        <c:axId val="1314665952"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1314612192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1314665952"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1314665952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1314612192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>336550</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>781050</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A6E3734-0480-1E4B-AF7F-E8182D9A89E3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Leighton Pritchard" refreshedDate="44480.685290162037" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="88">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:E89" sheet="esoph-tab"/>
+  </cacheSource>
+  <cacheFields count="5">
+    <cacheField name="agegp" numFmtId="49">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="alcgp" numFmtId="49">
+      <sharedItems count="4">
+        <s v="0-39"/>
+        <s v="40-79"/>
+        <s v="80-119"/>
+        <s v="120+"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="tobgp" numFmtId="49">
+      <sharedItems count="4">
+        <s v="0-9"/>
+        <s v="10-19"/>
+        <s v="20-29"/>
+        <s v="30+"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="ncases" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="17"/>
+    </cacheField>
+    <cacheField name="ncontrols" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="60"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="88">
+  <r>
+    <s v="25-34"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="40"/>
+  </r>
+  <r>
+    <s v="25-34"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="10"/>
+  </r>
+  <r>
+    <s v="25-34"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="0"/>
+    <n v="6"/>
+  </r>
+  <r>
+    <s v="25-34"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="0"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <s v="25-34"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="27"/>
+  </r>
+  <r>
+    <s v="25-34"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="7"/>
+  </r>
+  <r>
+    <s v="25-34"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <s v="25-34"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="0"/>
+    <n v="7"/>
+  </r>
+  <r>
+    <s v="25-34"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="25-34"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="25-34"/>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="0"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="25-34"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="25-34"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="25-34"/>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="25-34"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="0"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="35-44"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="60"/>
+  </r>
+  <r>
+    <s v="35-44"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="1"/>
+    <n v="14"/>
+  </r>
+  <r>
+    <s v="35-44"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="0"/>
+    <n v="7"/>
+  </r>
+  <r>
+    <s v="35-44"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="0"/>
+    <n v="8"/>
+  </r>
+  <r>
+    <s v="35-44"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="35"/>
+  </r>
+  <r>
+    <s v="35-44"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="3"/>
+    <n v="23"/>
+  </r>
+  <r>
+    <s v="35-44"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="14"/>
+  </r>
+  <r>
+    <s v="35-44"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="0"/>
+    <n v="8"/>
+  </r>
+  <r>
+    <s v="35-44"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="0"/>
+    <n v="11"/>
+  </r>
+  <r>
+    <s v="35-44"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="6"/>
+  </r>
+  <r>
+    <s v="35-44"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="0"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="35-44"/>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="35-44"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="2"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <s v="35-44"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <s v="35-44"/>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="2"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <s v="45-54"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="46"/>
+  </r>
+  <r>
+    <s v="45-54"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="18"/>
+  </r>
+  <r>
+    <s v="45-54"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="0"/>
+    <n v="10"/>
+  </r>
+  <r>
+    <s v="45-54"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="0"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <s v="45-54"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="6"/>
+    <n v="38"/>
+  </r>
+  <r>
+    <s v="45-54"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="4"/>
+    <n v="21"/>
+  </r>
+  <r>
+    <s v="45-54"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="5"/>
+    <n v="15"/>
+  </r>
+  <r>
+    <s v="45-54"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="5"/>
+    <n v="7"/>
+  </r>
+  <r>
+    <s v="45-54"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="3"/>
+    <n v="16"/>
+  </r>
+  <r>
+    <s v="45-54"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="6"/>
+    <n v="14"/>
+  </r>
+  <r>
+    <s v="45-54"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <s v="45-54"/>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="2"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <s v="45-54"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="4"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <s v="45-54"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="3"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <s v="45-54"/>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="2"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <s v="45-54"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="4"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <s v="55-64"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="2"/>
+    <n v="49"/>
+  </r>
+  <r>
+    <s v="55-64"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="3"/>
+    <n v="22"/>
+  </r>
+  <r>
+    <s v="55-64"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="3"/>
+    <n v="12"/>
+  </r>
+  <r>
+    <s v="55-64"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="4"/>
+    <n v="6"/>
+  </r>
+  <r>
+    <s v="55-64"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="9"/>
+    <n v="40"/>
+  </r>
+  <r>
+    <s v="55-64"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="6"/>
+    <n v="21"/>
+  </r>
+  <r>
+    <s v="55-64"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="4"/>
+    <n v="17"/>
+  </r>
+  <r>
+    <s v="55-64"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="3"/>
+    <n v="6"/>
+  </r>
+  <r>
+    <s v="55-64"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="9"/>
+    <n v="18"/>
+  </r>
+  <r>
+    <s v="55-64"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="8"/>
+    <n v="15"/>
+  </r>
+  <r>
+    <s v="55-64"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="3"/>
+    <n v="6"/>
+  </r>
+  <r>
+    <s v="55-64"/>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="4"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <s v="55-64"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="5"/>
+    <n v="10"/>
+  </r>
+  <r>
+    <s v="55-64"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="6"/>
+    <n v="7"/>
+  </r>
+  <r>
+    <s v="55-64"/>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="2"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <s v="55-64"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="5"/>
+    <n v="6"/>
+  </r>
+  <r>
+    <s v="65-74"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="5"/>
+    <n v="48"/>
+  </r>
+  <r>
+    <s v="65-74"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="4"/>
+    <n v="14"/>
+  </r>
+  <r>
+    <s v="65-74"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="2"/>
+    <n v="7"/>
+  </r>
+  <r>
+    <s v="65-74"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="0"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="65-74"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="17"/>
+    <n v="34"/>
+  </r>
+  <r>
+    <s v="65-74"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="3"/>
+    <n v="10"/>
+  </r>
+  <r>
+    <s v="65-74"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="5"/>
+    <n v="9"/>
+  </r>
+  <r>
+    <s v="65-74"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="6"/>
+    <n v="13"/>
+  </r>
+  <r>
+    <s v="65-74"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="4"/>
+    <n v="12"/>
+  </r>
+  <r>
+    <s v="65-74"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="2"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <s v="65-74"/>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="65-74"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="3"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <s v="65-74"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="1"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="65-74"/>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="65-74"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="75+"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="18"/>
+  </r>
+  <r>
+    <s v="75+"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="2"/>
+    <n v="6"/>
+  </r>
+  <r>
+    <s v="75+"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="1"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <s v="75+"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="2"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <s v="75+"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="1"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <s v="75+"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <s v="75+"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="75+"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="75+"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="75+"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="2"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="75+"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A3:C8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" sortType="ascending">
+      <items count="5">
+        <item x="0"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of ncases" fld="3" baseField="0" baseItem="0"/>
+    <dataField name="Sum of ncontrols" fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="2">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1011,13 +2783,103 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E90"/>
+  <dimension ref="A3:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="A90" sqref="A90"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2">
+        <v>29</v>
+      </c>
+      <c r="C4" s="2">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2">
+        <v>45</v>
+      </c>
+      <c r="C5" s="2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2">
+        <v>75</v>
+      </c>
+      <c r="C6" s="2">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2">
+        <v>51</v>
+      </c>
+      <c r="C7" s="2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="2">
+        <v>200</v>
+      </c>
+      <c r="C8" s="2">
+        <v>975</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K91"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E89"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="5" width="10.83203125" style="2"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -1029,10 +2891,10 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1046,11 +2908,11 @@
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1061,13 +2923,13 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
         <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1078,13 +2940,13 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1095,13 +2957,13 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1109,16 +2971,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>17</v>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1126,16 +2988,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>18</v>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1143,16 +3005,16 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>19</v>
+        <v>9</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1160,16 +3022,16 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1177,16 +3039,16 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>21</v>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1194,16 +3056,16 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>22</v>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1211,16 +3073,16 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1228,16 +3090,16 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>22</v>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1245,16 +3107,16 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>22</v>
+        <v>8</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1262,16 +3124,16 @@
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>22</v>
+        <v>9</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1279,21 +3141,21 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>6</v>
@@ -1301,254 +3163,254 @@
       <c r="C17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>25</v>
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2">
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>26</v>
+        <v>8</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2">
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2">
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2">
         <v>8</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>28</v>
+      <c r="D21" s="2">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2">
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>30</v>
+        <v>8</v>
+      </c>
+      <c r="D22" s="2">
+        <v>3</v>
+      </c>
+      <c r="E22" s="2">
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>26</v>
+        <v>9</v>
+      </c>
+      <c r="D23" s="2">
+        <v>1</v>
+      </c>
+      <c r="E23" s="2">
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2">
         <v>8</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>31</v>
+      <c r="D25" s="2">
+        <v>0</v>
+      </c>
+      <c r="E25" s="2">
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>13</v>
+      <c r="D26" s="2">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2">
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0</v>
+      </c>
+      <c r="E27" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>29</v>
+      <c r="D29" s="2">
+        <v>2</v>
+      </c>
+      <c r="E29" s="2">
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>29</v>
+      <c r="D30" s="2">
+        <v>0</v>
+      </c>
+      <c r="E30" s="2">
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>19</v>
+        <v>9</v>
+      </c>
+      <c r="D31" s="2">
+        <v>2</v>
+      </c>
+      <c r="E31" s="2">
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>6</v>
@@ -1556,271 +3418,271 @@
       <c r="C32" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>33</v>
+      <c r="D32" s="2">
+        <v>1</v>
+      </c>
+      <c r="E32" s="2">
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>34</v>
+      <c r="D33" s="2">
+        <v>0</v>
+      </c>
+      <c r="E33" s="2">
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0</v>
+      </c>
+      <c r="E34" s="2">
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0</v>
+      </c>
+      <c r="E35" s="2">
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>35</v>
+      <c r="D36" s="2">
+        <v>6</v>
+      </c>
+      <c r="E36" s="2">
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>36</v>
+        <v>8</v>
+      </c>
+      <c r="D37" s="2">
+        <v>4</v>
+      </c>
+      <c r="E37" s="2">
+        <v>21</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" s="2">
+        <v>5</v>
+      </c>
+      <c r="E38" s="2">
         <v>15</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="D39" s="2">
+        <v>5</v>
+      </c>
+      <c r="E39" s="2">
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>38</v>
+      <c r="D40" s="2">
+        <v>3</v>
+      </c>
+      <c r="E40" s="2">
+        <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>26</v>
+        <v>8</v>
+      </c>
+      <c r="D41" s="2">
+        <v>6</v>
+      </c>
+      <c r="E41" s="2">
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
+      </c>
+      <c r="D42" s="2">
+        <v>1</v>
+      </c>
+      <c r="E42" s="2">
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
+      </c>
+      <c r="D43" s="2">
+        <v>2</v>
+      </c>
+      <c r="E43" s="2">
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>19</v>
+      <c r="D44" s="2">
+        <v>4</v>
+      </c>
+      <c r="E44" s="2">
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
+      </c>
+      <c r="D45" s="2">
+        <v>3</v>
+      </c>
+      <c r="E45" s="2">
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>29</v>
+        <v>9</v>
+      </c>
+      <c r="D46" s="2">
+        <v>2</v>
+      </c>
+      <c r="E46" s="2">
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
+      </c>
+      <c r="D47" s="2">
+        <v>4</v>
+      </c>
+      <c r="E47" s="2">
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>6</v>
@@ -1828,271 +3690,271 @@
       <c r="C48" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>40</v>
+      <c r="D48" s="2">
+        <v>2</v>
+      </c>
+      <c r="E48" s="2">
+        <v>49</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>41</v>
+        <v>8</v>
+      </c>
+      <c r="D49" s="2">
+        <v>3</v>
+      </c>
+      <c r="E49" s="2">
+        <v>22</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C50" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" s="2">
+        <v>3</v>
+      </c>
+      <c r="E50" s="2">
         <v>12</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="D51" s="2">
+        <v>4</v>
+      </c>
+      <c r="E51" s="2">
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D52" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E52" s="1" t="s">
+      <c r="D52" s="2">
         <v>9</v>
+      </c>
+      <c r="E52" s="2">
+        <v>40</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>36</v>
+        <v>8</v>
+      </c>
+      <c r="D53" s="2">
+        <v>6</v>
+      </c>
+      <c r="E53" s="2">
+        <v>21</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>44</v>
+        <v>9</v>
+      </c>
+      <c r="D54" s="2">
+        <v>4</v>
+      </c>
+      <c r="E54" s="2">
+        <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="D55" s="2">
+        <v>3</v>
+      </c>
+      <c r="E55" s="2">
+        <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D56" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>34</v>
+      <c r="D56" s="2">
+        <v>9</v>
+      </c>
+      <c r="E56" s="2">
+        <v>18</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>37</v>
+        <v>8</v>
+      </c>
+      <c r="D57" s="2">
+        <v>8</v>
+      </c>
+      <c r="E57" s="2">
+        <v>15</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="D58" s="2">
+        <v>3</v>
+      </c>
+      <c r="E58" s="2">
+        <v>6</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
+      </c>
+      <c r="D59" s="2">
+        <v>4</v>
+      </c>
+      <c r="E59" s="2">
+        <v>4</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D60" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>11</v>
+      <c r="D60" s="2">
+        <v>5</v>
+      </c>
+      <c r="E60" s="2">
+        <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
+      </c>
+      <c r="D61" s="2">
+        <v>6</v>
+      </c>
+      <c r="E61" s="2">
+        <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>29</v>
+        <v>9</v>
+      </c>
+      <c r="D62" s="2">
+        <v>2</v>
+      </c>
+      <c r="E62" s="2">
+        <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="D63" s="2">
+        <v>5</v>
+      </c>
+      <c r="E63" s="2">
+        <v>6</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>6</v>
@@ -2100,254 +3962,254 @@
       <c r="C64" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D64" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>46</v>
+      <c r="D64" s="2">
+        <v>5</v>
+      </c>
+      <c r="E64" s="2">
+        <v>48</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>26</v>
+        <v>8</v>
+      </c>
+      <c r="D65" s="2">
+        <v>4</v>
+      </c>
+      <c r="E65" s="2">
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
+      </c>
+      <c r="D66" s="2">
+        <v>2</v>
+      </c>
+      <c r="E66" s="2">
+        <v>7</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
+      </c>
+      <c r="D67" s="2">
+        <v>0</v>
+      </c>
+      <c r="E67" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D68" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>47</v>
+      <c r="D68" s="2">
+        <v>17</v>
+      </c>
+      <c r="E68" s="2">
+        <v>34</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C69" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D69" s="2">
+        <v>3</v>
+      </c>
+      <c r="E69" s="2">
         <v>10</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>43</v>
+        <v>9</v>
+      </c>
+      <c r="D70" s="2">
+        <v>5</v>
+      </c>
+      <c r="E70" s="2">
+        <v>9</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D71" s="1" t="s">
+      <c r="D71" s="2">
+        <v>6</v>
+      </c>
+      <c r="E71" s="2">
         <v>13</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>42</v>
+        <v>8</v>
+      </c>
+      <c r="D72" s="2">
+        <v>4</v>
+      </c>
+      <c r="E72" s="2">
+        <v>12</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>29</v>
+        <v>9</v>
+      </c>
+      <c r="D73" s="2">
+        <v>2</v>
+      </c>
+      <c r="E73" s="2">
+        <v>3</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
+      </c>
+      <c r="D74" s="2">
+        <v>1</v>
+      </c>
+      <c r="E74" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D75" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>19</v>
+      <c r="D75" s="2">
+        <v>3</v>
+      </c>
+      <c r="E75" s="2">
+        <v>4</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>21</v>
+        <v>8</v>
+      </c>
+      <c r="D76" s="2">
+        <v>1</v>
+      </c>
+      <c r="E76" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>22</v>
+        <v>9</v>
+      </c>
+      <c r="D77" s="2">
+        <v>1</v>
+      </c>
+      <c r="E77" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
+      </c>
+      <c r="D78" s="2">
+        <v>1</v>
+      </c>
+      <c r="E78" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>6</v>
@@ -2355,185 +4217,209 @@
       <c r="C79" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D79" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>34</v>
+      <c r="D79" s="2">
+        <v>1</v>
+      </c>
+      <c r="E79" s="2">
+        <v>18</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="D80" s="2">
+        <v>2</v>
+      </c>
+      <c r="E80" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="D81" s="2">
+        <v>1</v>
+      </c>
+      <c r="E81" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D82" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D82" s="2">
+        <v>2</v>
+      </c>
+      <c r="E82" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C83" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D83" s="2">
+        <v>1</v>
+      </c>
+      <c r="E83" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D84" s="2">
+        <v>0</v>
+      </c>
+      <c r="E84" s="2">
+        <v>3</v>
+      </c>
+      <c r="K84" s="1"/>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C85" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D83" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A84" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C84" s="1" t="s">
+      <c r="D85" s="2">
+        <v>1</v>
+      </c>
+      <c r="E85" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B86" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A85" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A86" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D86" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D86" s="2">
+        <v>1</v>
+      </c>
+      <c r="E86" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="D87" s="2">
+        <v>1</v>
+      </c>
+      <c r="E87" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D88" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D88" s="2">
+        <v>2</v>
+      </c>
+      <c r="E88" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E89" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D90" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="D89" s="2">
+        <v>1</v>
+      </c>
+      <c r="E89" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C90" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D90" s="2">
+        <f>AVERAGE(D2:D89)</f>
+        <v>2.2727272727272729</v>
+      </c>
+      <c r="E90" s="2">
+        <f>AVERAGE(E2:E89)</f>
+        <v>11.079545454545455</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C91" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D91" s="2">
+        <f>STDEV(D2:D89)</f>
+        <v>2.7531685934710275</v>
+      </c>
+      <c r="E91" s="2">
+        <f>STDEV(E2:E89)</f>
+        <v>12.722702661361083</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>